<commit_message>
adding som progress for the array section
</commit_message>
<xml_diff>
--- a/monitor/FINAL450.xlsx
+++ b/monitor/FINAL450.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bernardocohen/repos/data_structures_algorithms/loving_babbar/monitor/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bernardocohen/repos/data_structures_algorithms/loving_babar/monitor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFB50A22-5BDE-5F4D-A460-1531FED01CCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC51B8FB-A87E-C344-9DE7-14B9A6932449}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="26880" windowHeight="16800" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1861,8 +1861,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1992,7 +1992,7 @@
         <v>14</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="21" x14ac:dyDescent="0.25">
@@ -2003,7 +2003,7 @@
         <v>15</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="21" x14ac:dyDescent="0.25">
@@ -2014,7 +2014,7 @@
         <v>16</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="21" x14ac:dyDescent="0.25">
@@ -2025,7 +2025,7 @@
         <v>17</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="21" x14ac:dyDescent="0.25">
@@ -2036,7 +2036,7 @@
         <v>18</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="21" x14ac:dyDescent="0.25">
@@ -2047,7 +2047,7 @@
         <v>19</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="21" x14ac:dyDescent="0.25">
@@ -2058,7 +2058,7 @@
         <v>20</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="21" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
working with array problems
</commit_message>
<xml_diff>
--- a/monitor/FINAL450.xlsx
+++ b/monitor/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bernardocohen/repos/data_structures_algorithms/loving_babar/monitor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC51B8FB-A87E-C344-9DE7-14B9A6932449}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD23820B-EA52-5B4C-97BB-7DC1D95CC9C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="26880" windowHeight="16800" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1861,8 +1861,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2069,7 +2069,7 @@
         <v>21</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="21" x14ac:dyDescent="0.25">
@@ -2080,7 +2080,7 @@
         <v>22</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="21" x14ac:dyDescent="0.25">
@@ -2091,7 +2091,7 @@
         <v>23</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="21" x14ac:dyDescent="0.25">
@@ -2102,7 +2102,7 @@
         <v>24</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="21" x14ac:dyDescent="0.25">
@@ -2113,7 +2113,7 @@
         <v>25</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="21" x14ac:dyDescent="0.25">
@@ -2124,7 +2124,7 @@
         <v>26</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="21" x14ac:dyDescent="0.25">
@@ -2135,7 +2135,7 @@
         <v>27</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="21" x14ac:dyDescent="0.25">
@@ -2146,7 +2146,7 @@
         <v>28</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="21" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
work with arrays section over :)
</commit_message>
<xml_diff>
--- a/monitor/FINAL450.xlsx
+++ b/monitor/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bernardocohen/repos/data_structures_algorithms/loving_babar/monitor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD23820B-EA52-5B4C-97BB-7DC1D95CC9C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC9E24B0-61BE-C441-9CA0-8E68F913F73F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="26880" windowHeight="16800" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1351" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1350" uniqueCount="467">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1429,13 +1429,16 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>redireccted to Check if all elements of the array are palindrome or not -&gt; both done</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1497,6 +1500,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1519,7 +1530,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1543,6 +1554,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1859,10 +1871,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C481"/>
+  <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="B27" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1870,6 +1882,7 @@
     <col min="1" max="1" width="28.5" customWidth="1"/>
     <col min="2" max="2" width="123" customWidth="1"/>
     <col min="3" max="3" width="27.5" customWidth="1"/>
+    <col min="4" max="4" width="71.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="26" x14ac:dyDescent="0.3">
@@ -2157,7 +2170,7 @@
         <v>29</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="21" x14ac:dyDescent="0.25">
@@ -2168,7 +2181,7 @@
         <v>30</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="21" x14ac:dyDescent="0.25">
@@ -2179,7 +2192,7 @@
         <v>31</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="21" x14ac:dyDescent="0.25">
@@ -2190,10 +2203,10 @@
         <v>32</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>5</v>
       </c>
@@ -2201,10 +2214,10 @@
         <v>33</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>5</v>
       </c>
@@ -2212,10 +2225,10 @@
         <v>34</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>5</v>
       </c>
@@ -2223,10 +2236,10 @@
         <v>35</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>5</v>
       </c>
@@ -2234,10 +2247,10 @@
         <v>36</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>5</v>
       </c>
@@ -2245,10 +2258,10 @@
         <v>37</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>5</v>
       </c>
@@ -2256,10 +2269,10 @@
         <v>38</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>5</v>
       </c>
@@ -2267,10 +2280,13 @@
         <v>39</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+        <v>465</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>5</v>
       </c>
@@ -2278,10 +2294,10 @@
         <v>40</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>5</v>
       </c>
@@ -2289,23 +2305,19 @@
         <v>41</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="B42" s="7"/>
-      <c r="C42" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="C42" s="4"/>
+    </row>
+    <row r="43" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A43" s="5"/>
       <c r="B43" s="7"/>
-      <c r="C43" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="C43" s="4"/>
+    </row>
+    <row r="44" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
         <v>42</v>
       </c>
@@ -2316,7 +2328,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
         <v>42</v>
       </c>
@@ -2327,7 +2339,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
         <v>42</v>
       </c>
@@ -2338,7 +2350,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
         <v>42</v>
       </c>
@@ -2349,7 +2361,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
         <v>42</v>
       </c>

</xml_diff>